<commit_message>
What we did in class 10/7
</commit_message>
<xml_diff>
--- a/ProgramPlanning.Wpf/Learning Outcomes.xlsx
+++ b/ProgramPlanning.Wpf/Learning Outcomes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20349"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20350"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c64a62ab78c248b/Documents/Snow/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ProgramPlanning\ProgramPlanning.Wpf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="8_{DB264028-D346-4F7C-B706-A93C98F052CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7AB09925-B4E8-49EC-86A7-14F96B2E32C1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A16B74-7C2A-463A-A58C-258F01353679}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="14100" xr2:uid="{736E1BEA-C0B9-40DD-8022-BD2245546042}"/>
   </bookViews>
@@ -561,6 +561,10 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D61D163-DDAA-4B95-8176-F89699E1E41A}" name="Table1" displayName="Table1" ref="A1:D142" totalsRowShown="0">
   <autoFilter ref="A1:D142" xr:uid="{1705DBE2-8C7E-4F78-90B2-A74D74893A95}"/>
+  <sortState ref="A2:D142">
+    <sortCondition ref="A2:A142"/>
+    <sortCondition ref="B2:B142"/>
+  </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{5119BF1B-9C29-4FEB-AC7E-8AB780AA86D7}" name="Area"/>
     <tableColumn id="2" xr3:uid="{BD0C2999-0259-4282-B66C-799935262D2F}" name="Course"/>
@@ -870,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F90E087-F363-4783-84FA-5A2E6F319782}">
   <dimension ref="A1:D142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -941,13 +945,13 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>1410</v>
+        <v>1400</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -961,7 +965,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -972,10 +976,10 @@
         <v>1410</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -983,13 +987,13 @@
         <v>2</v>
       </c>
       <c r="B8">
-        <v>1400</v>
+        <v>1410</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1347,13 +1351,13 @@
         <v>2</v>
       </c>
       <c r="B34">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1361,13 +1365,13 @@
         <v>2</v>
       </c>
       <c r="B35">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C35" t="s">
         <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1375,13 +1379,13 @@
         <v>2</v>
       </c>
       <c r="B36">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C36" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1395,7 +1399,7 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1409,7 +1413,7 @@
         <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1423,7 +1427,7 @@
         <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1437,7 +1441,7 @@
         <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1451,7 +1455,7 @@
         <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1462,10 +1466,10 @@
         <v>2450</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1473,13 +1477,13 @@
         <v>2</v>
       </c>
       <c r="B43">
-        <v>2420</v>
+        <v>2450</v>
       </c>
       <c r="C43" t="s">
         <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1487,13 +1491,13 @@
         <v>2</v>
       </c>
       <c r="B44">
-        <v>2420</v>
+        <v>2450</v>
       </c>
       <c r="C44" t="s">
         <v>3</v>
       </c>
       <c r="D44" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1501,13 +1505,13 @@
         <v>2</v>
       </c>
       <c r="B45">
-        <v>2420</v>
+        <v>2450</v>
       </c>
       <c r="C45" t="s">
         <v>10</v>
       </c>
       <c r="D45" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Rough data-driven diagram using course info
</commit_message>
<xml_diff>
--- a/ProgramPlanning.Wpf/Learning Outcomes.xlsx
+++ b/ProgramPlanning.Wpf/Learning Outcomes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ProgramPlanning\ProgramPlanning.Wpf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A16B74-7C2A-463A-A58C-258F01353679}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC5C66B-C221-4838-BBA7-7D8327E2A631}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="14100" xr2:uid="{736E1BEA-C0B9-40DD-8022-BD2245546042}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="184">
   <si>
     <t>Course</t>
   </si>
@@ -501,6 +501,129 @@
   </si>
   <si>
     <t>Students will demonstrate an ability to exercise and improve time and stress management skills as well as problem-solving skills.</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Programming Fundamentals</t>
+  </si>
+  <si>
+    <t>Prereq</t>
+  </si>
+  <si>
+    <t>Object-Oriented Programming</t>
+  </si>
+  <si>
+    <t>CS 1400</t>
+  </si>
+  <si>
+    <t>Coreq</t>
+  </si>
+  <si>
+    <t>CS 1415</t>
+  </si>
+  <si>
+    <t>Web Development I</t>
+  </si>
+  <si>
+    <t>CS 1410</t>
+  </si>
+  <si>
+    <t>Web Development II</t>
+  </si>
+  <si>
+    <t>CS 1810</t>
+  </si>
+  <si>
+    <t>Intro to Software Engineering</t>
+  </si>
+  <si>
+    <t>CS 2420</t>
+  </si>
+  <si>
+    <t>Data Structures and Algorithms</t>
+  </si>
+  <si>
+    <t>Computer Organization and Architecture</t>
+  </si>
+  <si>
+    <t>Web Development III</t>
+  </si>
+  <si>
+    <t>CS 1820</t>
+  </si>
+  <si>
+    <t>Operating Systems</t>
+  </si>
+  <si>
+    <t>CS 2810</t>
+  </si>
+  <si>
+    <t>Survey of Languages</t>
+  </si>
+  <si>
+    <t>Human Factors in Software Design</t>
+  </si>
+  <si>
+    <t>CS 2450</t>
+  </si>
+  <si>
+    <t>Principles and Patterns of Software Design</t>
+  </si>
+  <si>
+    <t>Database Systems</t>
+  </si>
+  <si>
+    <t>Distributed Application Development</t>
+  </si>
+  <si>
+    <t>SE 3520</t>
+  </si>
+  <si>
+    <t>CS 2860</t>
+  </si>
+  <si>
+    <t>Mobile Application Development</t>
+  </si>
+  <si>
+    <t>Management of Software Projects</t>
+  </si>
+  <si>
+    <t>SE 3410</t>
+  </si>
+  <si>
+    <t>Social and Ethical Issues in Computing</t>
+  </si>
+  <si>
+    <t>Graphical User Interfaces</t>
+  </si>
+  <si>
+    <t>SE 3250</t>
+  </si>
+  <si>
+    <t>Advanced Algorithms (Req MAT3310)</t>
+  </si>
+  <si>
+    <t>Personal Software Practices</t>
+  </si>
+  <si>
+    <t>SE 3450</t>
+  </si>
+  <si>
+    <t>Secure Coding Practices</t>
+  </si>
+  <si>
+    <t>SE 3620</t>
+  </si>
+  <si>
+    <t>Software Engineering Practicum I</t>
+  </si>
+  <si>
+    <t>Software Engineering Practicum II</t>
+  </si>
+  <si>
+    <t>SE 4400</t>
   </si>
 </sst>
 </file>
@@ -559,11 +682,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D61D163-DDAA-4B95-8176-F89699E1E41A}" name="Table1" displayName="Table1" ref="A1:D142" totalsRowShown="0">
-  <autoFilter ref="A1:D142" xr:uid="{1705DBE2-8C7E-4F78-90B2-A74D74893A95}"/>
-  <sortState ref="A2:D142">
-    <sortCondition ref="A2:A142"/>
-    <sortCondition ref="B2:B142"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D61D163-DDAA-4B95-8176-F89699E1E41A}" name="Table1" displayName="Table1" ref="A1:D191" totalsRowShown="0">
+  <autoFilter ref="A1:D191" xr:uid="{1705DBE2-8C7E-4F78-90B2-A74D74893A95}"/>
+  <sortState ref="A2:D191">
+    <sortCondition ref="A2:A191"/>
+    <sortCondition ref="B2:B191"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{5119BF1B-9C29-4FEB-AC7E-8AB780AA86D7}" name="Area"/>
@@ -872,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F90E087-F363-4783-84FA-5A2E6F319782}">
-  <dimension ref="A1:D142"/>
+  <dimension ref="A1:D191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="D177" sqref="D177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -959,13 +1082,13 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>1410</v>
+        <v>1400</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -979,7 +1102,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -990,10 +1113,10 @@
         <v>1410</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1001,13 +1124,13 @@
         <v>2</v>
       </c>
       <c r="B9">
-        <v>1810</v>
+        <v>1410</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1015,13 +1138,13 @@
         <v>2</v>
       </c>
       <c r="B10">
-        <v>1810</v>
+        <v>1410</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1029,13 +1152,13 @@
         <v>2</v>
       </c>
       <c r="B11">
-        <v>1810</v>
+        <v>1410</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1043,13 +1166,13 @@
         <v>2</v>
       </c>
       <c r="B12">
-        <v>1810</v>
+        <v>1410</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>148</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1063,7 +1186,7 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1077,7 +1200,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1091,7 +1214,7 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1105,7 +1228,7 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1119,7 +1242,7 @@
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1133,7 +1256,7 @@
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1147,7 +1270,7 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1161,7 +1284,7 @@
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1172,10 +1295,10 @@
         <v>1810</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1183,13 +1306,13 @@
         <v>2</v>
       </c>
       <c r="B22">
-        <v>1820</v>
+        <v>1810</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1197,13 +1320,13 @@
         <v>2</v>
       </c>
       <c r="B23">
-        <v>1820</v>
+        <v>1810</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1211,13 +1334,13 @@
         <v>2</v>
       </c>
       <c r="B24">
-        <v>1820</v>
+        <v>1810</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1225,13 +1348,13 @@
         <v>2</v>
       </c>
       <c r="B25">
-        <v>1820</v>
+        <v>1810</v>
       </c>
       <c r="C25" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1239,13 +1362,13 @@
         <v>2</v>
       </c>
       <c r="B26">
-        <v>1820</v>
+        <v>1810</v>
       </c>
       <c r="C26" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1253,13 +1376,13 @@
         <v>2</v>
       </c>
       <c r="B27">
-        <v>1820</v>
+        <v>1810</v>
       </c>
       <c r="C27" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D27" t="s">
-        <v>32</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1273,7 +1396,7 @@
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1287,7 +1410,7 @@
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1298,10 +1421,10 @@
         <v>1820</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1309,13 +1432,13 @@
         <v>2</v>
       </c>
       <c r="B31">
-        <v>2420</v>
+        <v>1820</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1323,13 +1446,13 @@
         <v>2</v>
       </c>
       <c r="B32">
-        <v>2420</v>
+        <v>1820</v>
       </c>
       <c r="C32" t="s">
         <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1337,13 +1460,13 @@
         <v>2</v>
       </c>
       <c r="B33">
-        <v>2420</v>
+        <v>1820</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1351,13 +1474,13 @@
         <v>2</v>
       </c>
       <c r="B34">
-        <v>2420</v>
+        <v>1820</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1365,13 +1488,13 @@
         <v>2</v>
       </c>
       <c r="B35">
-        <v>2420</v>
+        <v>1820</v>
       </c>
       <c r="C35" t="s">
         <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1379,13 +1502,13 @@
         <v>2</v>
       </c>
       <c r="B36">
-        <v>2420</v>
+        <v>1820</v>
       </c>
       <c r="C36" t="s">
         <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1393,13 +1516,13 @@
         <v>2</v>
       </c>
       <c r="B37">
-        <v>2450</v>
+        <v>1820</v>
       </c>
       <c r="C37" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D37" t="s">
-        <v>39</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1407,13 +1530,13 @@
         <v>2</v>
       </c>
       <c r="B38">
-        <v>2450</v>
+        <v>1820</v>
       </c>
       <c r="C38" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D38" t="s">
-        <v>40</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1421,13 +1544,13 @@
         <v>2</v>
       </c>
       <c r="B39">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C39" t="s">
         <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1435,13 +1558,13 @@
         <v>2</v>
       </c>
       <c r="B40">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C40" t="s">
         <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1449,13 +1572,13 @@
         <v>2</v>
       </c>
       <c r="B41">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C41" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1463,13 +1586,13 @@
         <v>2</v>
       </c>
       <c r="B42">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C42" t="s">
         <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1477,13 +1600,13 @@
         <v>2</v>
       </c>
       <c r="B43">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C43" t="s">
         <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1491,13 +1614,13 @@
         <v>2</v>
       </c>
       <c r="B44">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C44" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1505,13 +1628,13 @@
         <v>2</v>
       </c>
       <c r="B45">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C45" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="D45" t="s">
-        <v>47</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1519,13 +1642,13 @@
         <v>2</v>
       </c>
       <c r="B46">
-        <v>2810</v>
+        <v>2420</v>
       </c>
       <c r="C46" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D46" t="s">
-        <v>48</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1533,13 +1656,13 @@
         <v>2</v>
       </c>
       <c r="B47">
-        <v>2810</v>
+        <v>2450</v>
       </c>
       <c r="C47" t="s">
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1547,13 +1670,13 @@
         <v>2</v>
       </c>
       <c r="B48">
-        <v>2810</v>
+        <v>2450</v>
       </c>
       <c r="C48" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1561,13 +1684,13 @@
         <v>2</v>
       </c>
       <c r="B49">
-        <v>2830</v>
+        <v>2450</v>
       </c>
       <c r="C49" t="s">
         <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1575,13 +1698,13 @@
         <v>2</v>
       </c>
       <c r="B50">
-        <v>2830</v>
+        <v>2450</v>
       </c>
       <c r="C50" t="s">
         <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1589,13 +1712,13 @@
         <v>2</v>
       </c>
       <c r="B51">
-        <v>2830</v>
+        <v>2450</v>
       </c>
       <c r="C51" t="s">
         <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1603,13 +1726,13 @@
         <v>2</v>
       </c>
       <c r="B52">
-        <v>2830</v>
+        <v>2450</v>
       </c>
       <c r="C52" t="s">
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1617,13 +1740,13 @@
         <v>2</v>
       </c>
       <c r="B53">
-        <v>2830</v>
+        <v>2450</v>
       </c>
       <c r="C53" t="s">
         <v>3</v>
       </c>
       <c r="D53" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1631,13 +1754,13 @@
         <v>2</v>
       </c>
       <c r="B54">
-        <v>2830</v>
+        <v>2450</v>
       </c>
       <c r="C54" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1645,13 +1768,13 @@
         <v>2</v>
       </c>
       <c r="B55">
-        <v>2860</v>
+        <v>2450</v>
       </c>
       <c r="C55" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1659,13 +1782,13 @@
         <v>2</v>
       </c>
       <c r="B56">
-        <v>2860</v>
+        <v>2450</v>
       </c>
       <c r="C56" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D56" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1673,13 +1796,13 @@
         <v>2</v>
       </c>
       <c r="B57">
-        <v>2860</v>
+        <v>2450</v>
       </c>
       <c r="C57" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D57" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1687,13 +1810,13 @@
         <v>2</v>
       </c>
       <c r="B58">
-        <v>2860</v>
+        <v>2810</v>
       </c>
       <c r="C58" t="s">
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1701,13 +1824,13 @@
         <v>2</v>
       </c>
       <c r="B59">
-        <v>2860</v>
+        <v>2810</v>
       </c>
       <c r="C59" t="s">
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1715,13 +1838,13 @@
         <v>2</v>
       </c>
       <c r="B60">
-        <v>2860</v>
+        <v>2810</v>
       </c>
       <c r="C60" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1729,13 +1852,13 @@
         <v>2</v>
       </c>
       <c r="B61">
-        <v>2860</v>
+        <v>2810</v>
       </c>
       <c r="C61" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D61" t="s">
-        <v>63</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1743,13 +1866,13 @@
         <v>2</v>
       </c>
       <c r="B62">
-        <v>2860</v>
+        <v>2810</v>
       </c>
       <c r="C62" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D62" t="s">
-        <v>64</v>
+        <v>155</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1757,293 +1880,293 @@
         <v>2</v>
       </c>
       <c r="B63">
-        <v>2860</v>
+        <v>2830</v>
       </c>
       <c r="C63" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B64">
-        <v>3250</v>
+        <v>2830</v>
       </c>
       <c r="C64" t="s">
         <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B65">
-        <v>3250</v>
+        <v>2830</v>
       </c>
       <c r="C65" t="s">
         <v>3</v>
       </c>
       <c r="D65" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B66">
-        <v>3250</v>
+        <v>2830</v>
       </c>
       <c r="C66" t="s">
         <v>3</v>
       </c>
       <c r="D66" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B67">
-        <v>3250</v>
+        <v>2830</v>
       </c>
       <c r="C67" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B68">
-        <v>3410</v>
+        <v>2830</v>
       </c>
       <c r="C68" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D68" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B69">
-        <v>3410</v>
+        <v>2830</v>
       </c>
       <c r="C69" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D69" t="s">
-        <v>72</v>
+        <v>158</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B70">
-        <v>3410</v>
+        <v>2830</v>
       </c>
       <c r="C70" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D70" t="s">
-        <v>73</v>
+        <v>159</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B71">
-        <v>3410</v>
+        <v>2860</v>
       </c>
       <c r="C71" t="s">
         <v>3</v>
       </c>
       <c r="D71" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B72">
-        <v>3410</v>
+        <v>2860</v>
       </c>
       <c r="C72" t="s">
         <v>3</v>
       </c>
       <c r="D72" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B73">
-        <v>3410</v>
+        <v>2860</v>
       </c>
       <c r="C73" t="s">
         <v>3</v>
       </c>
       <c r="D73" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B74">
-        <v>3410</v>
+        <v>2860</v>
       </c>
       <c r="C74" t="s">
         <v>3</v>
       </c>
       <c r="D74" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B75">
-        <v>3410</v>
+        <v>2860</v>
       </c>
       <c r="C75" t="s">
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B76">
-        <v>3410</v>
+        <v>2860</v>
       </c>
       <c r="C76" t="s">
         <v>3</v>
       </c>
       <c r="D76" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B77">
-        <v>3410</v>
+        <v>2860</v>
       </c>
       <c r="C77" t="s">
         <v>3</v>
       </c>
       <c r="D77" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B78">
-        <v>3410</v>
+        <v>2860</v>
       </c>
       <c r="C78" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D78" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B79">
-        <v>3450</v>
+        <v>2860</v>
       </c>
       <c r="C79" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D79" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B80">
-        <v>3450</v>
+        <v>2860</v>
       </c>
       <c r="C80" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D80" t="s">
-        <v>83</v>
+        <v>160</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B81">
-        <v>3450</v>
+        <v>2860</v>
       </c>
       <c r="C81" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D81" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B82">
-        <v>3450</v>
+        <v>3250</v>
       </c>
       <c r="C82" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="D82" t="s">
-        <v>85</v>
+        <v>162</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B83">
-        <v>3520</v>
+        <v>3250</v>
       </c>
       <c r="C83" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D83" t="s">
-        <v>86</v>
+        <v>155</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -2051,13 +2174,13 @@
         <v>66</v>
       </c>
       <c r="B84">
-        <v>3520</v>
+        <v>3250</v>
       </c>
       <c r="C84" t="s">
         <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -2065,13 +2188,13 @@
         <v>66</v>
       </c>
       <c r="B85">
-        <v>3520</v>
+        <v>3250</v>
       </c>
       <c r="C85" t="s">
         <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -2079,13 +2202,13 @@
         <v>66</v>
       </c>
       <c r="B86">
-        <v>3520</v>
+        <v>3250</v>
       </c>
       <c r="C86" t="s">
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -2093,13 +2216,13 @@
         <v>66</v>
       </c>
       <c r="B87">
-        <v>3520</v>
+        <v>3250</v>
       </c>
       <c r="C87" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D87" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -2107,13 +2230,13 @@
         <v>66</v>
       </c>
       <c r="B88">
-        <v>3520</v>
+        <v>3410</v>
       </c>
       <c r="C88" t="s">
         <v>3</v>
       </c>
       <c r="D88" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -2121,13 +2244,13 @@
         <v>66</v>
       </c>
       <c r="B89">
-        <v>3520</v>
+        <v>3410</v>
       </c>
       <c r="C89" t="s">
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -2135,13 +2258,13 @@
         <v>66</v>
       </c>
       <c r="B90">
-        <v>3520</v>
+        <v>3410</v>
       </c>
       <c r="C90" t="s">
         <v>3</v>
       </c>
       <c r="D90" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -2149,13 +2272,13 @@
         <v>66</v>
       </c>
       <c r="B91">
-        <v>3520</v>
+        <v>3410</v>
       </c>
       <c r="C91" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D91" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -2163,13 +2286,13 @@
         <v>66</v>
       </c>
       <c r="B92">
-        <v>3620</v>
+        <v>3410</v>
       </c>
       <c r="C92" t="s">
         <v>3</v>
       </c>
       <c r="D92" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -2177,13 +2300,13 @@
         <v>66</v>
       </c>
       <c r="B93">
-        <v>3620</v>
+        <v>3410</v>
       </c>
       <c r="C93" t="s">
         <v>3</v>
       </c>
       <c r="D93" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -2191,13 +2314,13 @@
         <v>66</v>
       </c>
       <c r="B94">
-        <v>3620</v>
+        <v>3410</v>
       </c>
       <c r="C94" t="s">
         <v>3</v>
       </c>
       <c r="D94" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -2205,13 +2328,13 @@
         <v>66</v>
       </c>
       <c r="B95">
-        <v>3620</v>
+        <v>3410</v>
       </c>
       <c r="C95" t="s">
         <v>3</v>
       </c>
       <c r="D95" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -2219,13 +2342,13 @@
         <v>66</v>
       </c>
       <c r="B96">
-        <v>3620</v>
+        <v>3410</v>
       </c>
       <c r="C96" t="s">
         <v>3</v>
       </c>
       <c r="D96" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -2233,13 +2356,13 @@
         <v>66</v>
       </c>
       <c r="B97">
-        <v>3620</v>
+        <v>3410</v>
       </c>
       <c r="C97" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D97" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -2247,13 +2370,13 @@
         <v>66</v>
       </c>
       <c r="B98">
-        <v>3630</v>
+        <v>3410</v>
       </c>
       <c r="C98" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D98" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -2261,13 +2384,13 @@
         <v>66</v>
       </c>
       <c r="B99">
-        <v>3630</v>
+        <v>3410</v>
       </c>
       <c r="C99" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D99" t="s">
-        <v>102</v>
+        <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -2275,13 +2398,13 @@
         <v>66</v>
       </c>
       <c r="B100">
-        <v>3630</v>
+        <v>3410</v>
       </c>
       <c r="C100" t="s">
-        <v>10</v>
+        <v>145</v>
       </c>
       <c r="D100" t="s">
-        <v>103</v>
+        <v>164</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -2289,13 +2412,13 @@
         <v>66</v>
       </c>
       <c r="B101">
-        <v>4120</v>
+        <v>3450</v>
       </c>
       <c r="C101" t="s">
         <v>3</v>
       </c>
       <c r="D101" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -2303,13 +2426,13 @@
         <v>66</v>
       </c>
       <c r="B102">
-        <v>4120</v>
+        <v>3450</v>
       </c>
       <c r="C102" t="s">
         <v>3</v>
       </c>
       <c r="D102" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -2317,13 +2440,13 @@
         <v>66</v>
       </c>
       <c r="B103">
-        <v>4120</v>
+        <v>3450</v>
       </c>
       <c r="C103" t="s">
         <v>3</v>
       </c>
       <c r="D103" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -2331,13 +2454,13 @@
         <v>66</v>
       </c>
       <c r="B104">
-        <v>4120</v>
+        <v>3450</v>
       </c>
       <c r="C104" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D104" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -2345,13 +2468,13 @@
         <v>66</v>
       </c>
       <c r="B105">
-        <v>4120</v>
+        <v>3450</v>
       </c>
       <c r="C105" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D105" t="s">
-        <v>108</v>
+        <v>165</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -2359,13 +2482,13 @@
         <v>66</v>
       </c>
       <c r="B106">
-        <v>4120</v>
+        <v>3450</v>
       </c>
       <c r="C106" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D106" t="s">
-        <v>109</v>
+        <v>164</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -2373,13 +2496,13 @@
         <v>66</v>
       </c>
       <c r="B107">
-        <v>4120</v>
+        <v>3520</v>
       </c>
       <c r="C107" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D107" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -2387,13 +2510,13 @@
         <v>66</v>
       </c>
       <c r="B108">
-        <v>4140</v>
+        <v>3520</v>
       </c>
       <c r="C108" t="s">
         <v>3</v>
       </c>
       <c r="D108" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -2401,13 +2524,13 @@
         <v>66</v>
       </c>
       <c r="B109">
-        <v>4140</v>
+        <v>3520</v>
       </c>
       <c r="C109" t="s">
         <v>3</v>
       </c>
       <c r="D109" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
@@ -2415,13 +2538,13 @@
         <v>66</v>
       </c>
       <c r="B110">
-        <v>4140</v>
+        <v>3520</v>
       </c>
       <c r="C110" t="s">
         <v>3</v>
       </c>
       <c r="D110" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -2429,13 +2552,13 @@
         <v>66</v>
       </c>
       <c r="B111">
-        <v>4140</v>
+        <v>3520</v>
       </c>
       <c r="C111" t="s">
         <v>3</v>
       </c>
       <c r="D111" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
@@ -2443,13 +2566,13 @@
         <v>66</v>
       </c>
       <c r="B112">
-        <v>4140</v>
+        <v>3520</v>
       </c>
       <c r="C112" t="s">
         <v>3</v>
       </c>
       <c r="D112" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
@@ -2457,27 +2580,27 @@
         <v>66</v>
       </c>
       <c r="B113">
-        <v>4140</v>
+        <v>3520</v>
       </c>
       <c r="C113" t="s">
         <v>3</v>
       </c>
       <c r="D113" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>66</v>
       </c>
       <c r="B114">
-        <v>4140</v>
+        <v>3520</v>
       </c>
       <c r="C114" t="s">
-        <v>10</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>117</v>
+        <v>3</v>
+      </c>
+      <c r="D114" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
@@ -2485,13 +2608,13 @@
         <v>66</v>
       </c>
       <c r="B115">
-        <v>4220</v>
+        <v>3520</v>
       </c>
       <c r="C115" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D115" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
@@ -2499,13 +2622,13 @@
         <v>66</v>
       </c>
       <c r="B116">
-        <v>4220</v>
+        <v>3520</v>
       </c>
       <c r="C116" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D116" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
@@ -2513,27 +2636,27 @@
         <v>66</v>
       </c>
       <c r="B117">
-        <v>4220</v>
+        <v>3520</v>
       </c>
       <c r="C117" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D117" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="302.39999999999998" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>66</v>
       </c>
       <c r="B118">
-        <v>4220</v>
+        <v>3620</v>
       </c>
       <c r="C118" t="s">
-        <v>10</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>121</v>
+        <v>3</v>
+      </c>
+      <c r="D118" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
@@ -2541,13 +2664,13 @@
         <v>66</v>
       </c>
       <c r="B119">
-        <v>4230</v>
+        <v>3620</v>
       </c>
       <c r="C119" t="s">
         <v>3</v>
       </c>
       <c r="D119" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
@@ -2555,13 +2678,13 @@
         <v>66</v>
       </c>
       <c r="B120">
-        <v>4230</v>
+        <v>3620</v>
       </c>
       <c r="C120" t="s">
         <v>3</v>
       </c>
       <c r="D120" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -2569,13 +2692,13 @@
         <v>66</v>
       </c>
       <c r="B121">
-        <v>4230</v>
+        <v>3620</v>
       </c>
       <c r="C121" t="s">
         <v>3</v>
       </c>
       <c r="D121" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
@@ -2583,13 +2706,13 @@
         <v>66</v>
       </c>
       <c r="B122">
-        <v>4230</v>
+        <v>3620</v>
       </c>
       <c r="C122" t="s">
         <v>3</v>
       </c>
       <c r="D122" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
@@ -2597,13 +2720,13 @@
         <v>66</v>
       </c>
       <c r="B123">
-        <v>4230</v>
+        <v>3620</v>
       </c>
       <c r="C123" t="s">
         <v>10</v>
       </c>
       <c r="D123" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
@@ -2611,13 +2734,13 @@
         <v>66</v>
       </c>
       <c r="B124">
-        <v>4320</v>
+        <v>3620</v>
       </c>
       <c r="C124" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D124" t="s">
-        <v>127</v>
+        <v>167</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
@@ -2625,13 +2748,13 @@
         <v>66</v>
       </c>
       <c r="B125">
-        <v>4320</v>
+        <v>3620</v>
       </c>
       <c r="C125" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D125" t="s">
-        <v>128</v>
+        <v>168</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
@@ -2639,13 +2762,13 @@
         <v>66</v>
       </c>
       <c r="B126">
-        <v>4320</v>
+        <v>3620</v>
       </c>
       <c r="C126" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D126" t="s">
-        <v>129</v>
+        <v>169</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
@@ -2653,27 +2776,27 @@
         <v>66</v>
       </c>
       <c r="B127">
-        <v>4320</v>
+        <v>3630</v>
       </c>
       <c r="C127" t="s">
         <v>3</v>
       </c>
       <c r="D127" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>66</v>
       </c>
       <c r="B128">
-        <v>4320</v>
+        <v>3630</v>
       </c>
       <c r="C128" t="s">
-        <v>10</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>131</v>
+        <v>3</v>
+      </c>
+      <c r="D128" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
@@ -2681,13 +2804,13 @@
         <v>66</v>
       </c>
       <c r="B129">
-        <v>4340</v>
+        <v>3630</v>
       </c>
       <c r="C129" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D129" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
@@ -2695,13 +2818,13 @@
         <v>66</v>
       </c>
       <c r="B130">
-        <v>4340</v>
+        <v>3630</v>
       </c>
       <c r="C130" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D130" t="s">
-        <v>133</v>
+        <v>170</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
@@ -2709,13 +2832,13 @@
         <v>66</v>
       </c>
       <c r="B131">
-        <v>4340</v>
+        <v>3630</v>
       </c>
       <c r="C131" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D131" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
@@ -2723,13 +2846,13 @@
         <v>66</v>
       </c>
       <c r="B132">
-        <v>4340</v>
+        <v>4120</v>
       </c>
       <c r="C132" t="s">
         <v>3</v>
       </c>
       <c r="D132" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
@@ -2737,27 +2860,27 @@
         <v>66</v>
       </c>
       <c r="B133">
-        <v>4340</v>
+        <v>4120</v>
       </c>
       <c r="C133" t="s">
         <v>3</v>
       </c>
       <c r="D133" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>66</v>
       </c>
       <c r="B134">
-        <v>4340</v>
+        <v>4120</v>
       </c>
       <c r="C134" t="s">
-        <v>10</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>137</v>
+        <v>3</v>
+      </c>
+      <c r="D134" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
@@ -2765,13 +2888,13 @@
         <v>66</v>
       </c>
       <c r="B135">
-        <v>4400</v>
+        <v>4120</v>
       </c>
       <c r="C135" t="s">
         <v>3</v>
       </c>
       <c r="D135" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
@@ -2779,13 +2902,13 @@
         <v>66</v>
       </c>
       <c r="B136">
-        <v>4400</v>
+        <v>4120</v>
       </c>
       <c r="C136" t="s">
         <v>3</v>
       </c>
       <c r="D136" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
@@ -2793,13 +2916,13 @@
         <v>66</v>
       </c>
       <c r="B137">
-        <v>4400</v>
+        <v>4120</v>
       </c>
       <c r="C137" t="s">
         <v>3</v>
       </c>
       <c r="D137" t="s">
-        <v>140</v>
+        <v>109</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
@@ -2807,13 +2930,13 @@
         <v>66</v>
       </c>
       <c r="B138">
-        <v>4400</v>
+        <v>4120</v>
       </c>
       <c r="C138" t="s">
         <v>10</v>
       </c>
       <c r="D138" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
@@ -2821,13 +2944,13 @@
         <v>66</v>
       </c>
       <c r="B139">
-        <v>4450</v>
+        <v>4120</v>
       </c>
       <c r="C139" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D139" t="s">
-        <v>138</v>
+        <v>171</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
@@ -2835,13 +2958,13 @@
         <v>66</v>
       </c>
       <c r="B140">
-        <v>4450</v>
+        <v>4120</v>
       </c>
       <c r="C140" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D140" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
@@ -2849,13 +2972,13 @@
         <v>66</v>
       </c>
       <c r="B141">
-        <v>4450</v>
+        <v>4140</v>
       </c>
       <c r="C141" t="s">
         <v>3</v>
       </c>
       <c r="D141" t="s">
-        <v>142</v>
+        <v>111</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
@@ -2863,13 +2986,699 @@
         <v>66</v>
       </c>
       <c r="B142">
+        <v>4140</v>
+      </c>
+      <c r="C142" t="s">
+        <v>3</v>
+      </c>
+      <c r="D142" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>66</v>
+      </c>
+      <c r="B143">
+        <v>4140</v>
+      </c>
+      <c r="C143" t="s">
+        <v>3</v>
+      </c>
+      <c r="D143" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>66</v>
+      </c>
+      <c r="B144">
+        <v>4140</v>
+      </c>
+      <c r="C144" t="s">
+        <v>3</v>
+      </c>
+      <c r="D144" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>66</v>
+      </c>
+      <c r="B145">
+        <v>4140</v>
+      </c>
+      <c r="C145" t="s">
+        <v>3</v>
+      </c>
+      <c r="D145" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>66</v>
+      </c>
+      <c r="B146">
+        <v>4140</v>
+      </c>
+      <c r="C146" t="s">
+        <v>3</v>
+      </c>
+      <c r="D146" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>66</v>
+      </c>
+      <c r="B147">
+        <v>4140</v>
+      </c>
+      <c r="C147" t="s">
+        <v>10</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>66</v>
+      </c>
+      <c r="B148">
+        <v>4140</v>
+      </c>
+      <c r="C148" t="s">
+        <v>143</v>
+      </c>
+      <c r="D148" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>66</v>
+      </c>
+      <c r="B149">
+        <v>4140</v>
+      </c>
+      <c r="C149" t="s">
+        <v>145</v>
+      </c>
+      <c r="D149" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>66</v>
+      </c>
+      <c r="B150">
+        <v>4220</v>
+      </c>
+      <c r="C150" t="s">
+        <v>3</v>
+      </c>
+      <c r="D150" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>66</v>
+      </c>
+      <c r="B151">
+        <v>4220</v>
+      </c>
+      <c r="C151" t="s">
+        <v>3</v>
+      </c>
+      <c r="D151" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>66</v>
+      </c>
+      <c r="B152">
+        <v>4220</v>
+      </c>
+      <c r="C152" t="s">
+        <v>3</v>
+      </c>
+      <c r="D152" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>66</v>
+      </c>
+      <c r="B153">
+        <v>4220</v>
+      </c>
+      <c r="C153" t="s">
+        <v>10</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>66</v>
+      </c>
+      <c r="B154">
+        <v>4220</v>
+      </c>
+      <c r="C154" t="s">
+        <v>143</v>
+      </c>
+      <c r="D154" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>66</v>
+      </c>
+      <c r="B155">
+        <v>4220</v>
+      </c>
+      <c r="C155" t="s">
+        <v>145</v>
+      </c>
+      <c r="D155" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>66</v>
+      </c>
+      <c r="B156">
+        <v>4220</v>
+      </c>
+      <c r="C156" t="s">
+        <v>145</v>
+      </c>
+      <c r="D156" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>66</v>
+      </c>
+      <c r="B157">
+        <v>4230</v>
+      </c>
+      <c r="C157" t="s">
+        <v>3</v>
+      </c>
+      <c r="D157" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>66</v>
+      </c>
+      <c r="B158">
+        <v>4230</v>
+      </c>
+      <c r="C158" t="s">
+        <v>3</v>
+      </c>
+      <c r="D158" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>66</v>
+      </c>
+      <c r="B159">
+        <v>4230</v>
+      </c>
+      <c r="C159" t="s">
+        <v>3</v>
+      </c>
+      <c r="D159" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>66</v>
+      </c>
+      <c r="B160">
+        <v>4230</v>
+      </c>
+      <c r="C160" t="s">
+        <v>3</v>
+      </c>
+      <c r="D160" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>66</v>
+      </c>
+      <c r="B161">
+        <v>4230</v>
+      </c>
+      <c r="C161" t="s">
+        <v>10</v>
+      </c>
+      <c r="D161" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>66</v>
+      </c>
+      <c r="B162">
+        <v>4230</v>
+      </c>
+      <c r="C162" t="s">
+        <v>143</v>
+      </c>
+      <c r="D162" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>66</v>
+      </c>
+      <c r="B163">
+        <v>4230</v>
+      </c>
+      <c r="C163" t="s">
+        <v>145</v>
+      </c>
+      <c r="D163" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>66</v>
+      </c>
+      <c r="B164">
+        <v>4320</v>
+      </c>
+      <c r="C164" t="s">
+        <v>3</v>
+      </c>
+      <c r="D164" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>66</v>
+      </c>
+      <c r="B165">
+        <v>4320</v>
+      </c>
+      <c r="C165" t="s">
+        <v>3</v>
+      </c>
+      <c r="D165" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>66</v>
+      </c>
+      <c r="B166">
+        <v>4320</v>
+      </c>
+      <c r="C166" t="s">
+        <v>3</v>
+      </c>
+      <c r="D166" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>66</v>
+      </c>
+      <c r="B167">
+        <v>4320</v>
+      </c>
+      <c r="C167" t="s">
+        <v>3</v>
+      </c>
+      <c r="D167" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>66</v>
+      </c>
+      <c r="B168">
+        <v>4320</v>
+      </c>
+      <c r="C168" t="s">
+        <v>10</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>66</v>
+      </c>
+      <c r="B169">
+        <v>4320</v>
+      </c>
+      <c r="C169" t="s">
+        <v>143</v>
+      </c>
+      <c r="D169" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>66</v>
+      </c>
+      <c r="B170">
+        <v>4320</v>
+      </c>
+      <c r="C170" t="s">
+        <v>145</v>
+      </c>
+      <c r="D170" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>66</v>
+      </c>
+      <c r="B171">
+        <v>4340</v>
+      </c>
+      <c r="C171" t="s">
+        <v>3</v>
+      </c>
+      <c r="D171" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>66</v>
+      </c>
+      <c r="B172">
+        <v>4340</v>
+      </c>
+      <c r="C172" t="s">
+        <v>3</v>
+      </c>
+      <c r="D172" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>66</v>
+      </c>
+      <c r="B173">
+        <v>4340</v>
+      </c>
+      <c r="C173" t="s">
+        <v>3</v>
+      </c>
+      <c r="D173" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>66</v>
+      </c>
+      <c r="B174">
+        <v>4340</v>
+      </c>
+      <c r="C174" t="s">
+        <v>3</v>
+      </c>
+      <c r="D174" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>66</v>
+      </c>
+      <c r="B175">
+        <v>4340</v>
+      </c>
+      <c r="C175" t="s">
+        <v>3</v>
+      </c>
+      <c r="D175" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>66</v>
+      </c>
+      <c r="B176">
+        <v>4340</v>
+      </c>
+      <c r="C176" t="s">
+        <v>10</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>66</v>
+      </c>
+      <c r="B177">
+        <v>4340</v>
+      </c>
+      <c r="C177" t="s">
+        <v>143</v>
+      </c>
+      <c r="D177" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>66</v>
+      </c>
+      <c r="B178">
+        <v>4340</v>
+      </c>
+      <c r="C178" t="s">
+        <v>145</v>
+      </c>
+      <c r="D178" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>66</v>
+      </c>
+      <c r="B179">
+        <v>4400</v>
+      </c>
+      <c r="C179" t="s">
+        <v>3</v>
+      </c>
+      <c r="D179" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>66</v>
+      </c>
+      <c r="B180">
+        <v>4400</v>
+      </c>
+      <c r="C180" t="s">
+        <v>3</v>
+      </c>
+      <c r="D180" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>66</v>
+      </c>
+      <c r="B181">
+        <v>4400</v>
+      </c>
+      <c r="C181" t="s">
+        <v>3</v>
+      </c>
+      <c r="D181" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>66</v>
+      </c>
+      <c r="B182">
+        <v>4400</v>
+      </c>
+      <c r="C182" t="s">
+        <v>10</v>
+      </c>
+      <c r="D182" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>66</v>
+      </c>
+      <c r="B183">
+        <v>4400</v>
+      </c>
+      <c r="C183" t="s">
+        <v>143</v>
+      </c>
+      <c r="D183" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>66</v>
+      </c>
+      <c r="B184">
+        <v>4400</v>
+      </c>
+      <c r="C184" t="s">
+        <v>145</v>
+      </c>
+      <c r="D184" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>66</v>
+      </c>
+      <c r="B185">
+        <v>4400</v>
+      </c>
+      <c r="C185" t="s">
+        <v>145</v>
+      </c>
+      <c r="D185" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>66</v>
+      </c>
+      <c r="B186">
         <v>4450</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C186" t="s">
+        <v>3</v>
+      </c>
+      <c r="D186" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>66</v>
+      </c>
+      <c r="B187">
+        <v>4450</v>
+      </c>
+      <c r="C187" t="s">
+        <v>3</v>
+      </c>
+      <c r="D187" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>66</v>
+      </c>
+      <c r="B188">
+        <v>4450</v>
+      </c>
+      <c r="C188" t="s">
+        <v>3</v>
+      </c>
+      <c r="D188" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>66</v>
+      </c>
+      <c r="B189">
+        <v>4450</v>
+      </c>
+      <c r="C189" t="s">
         <v>10</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D189" t="s">
         <v>141</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>66</v>
+      </c>
+      <c r="B190">
+        <v>4450</v>
+      </c>
+      <c r="C190" t="s">
+        <v>143</v>
+      </c>
+      <c r="D190" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>66</v>
+      </c>
+      <c r="B191">
+        <v>4450</v>
+      </c>
+      <c r="C191" t="s">
+        <v>145</v>
+      </c>
+      <c r="D191" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Better handle prerequisites, add export to png, include semester info
</commit_message>
<xml_diff>
--- a/ProgramPlanning.Wpf/Learning Outcomes.xlsx
+++ b/ProgramPlanning.Wpf/Learning Outcomes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ProgramPlanning\ProgramPlanning.Wpf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC5C66B-C221-4838-BBA7-7D8327E2A631}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08137168-8772-4CE0-8333-062C90CB003C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="14100" xr2:uid="{736E1BEA-C0B9-40DD-8022-BD2245546042}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="221">
   <si>
     <t>Course</t>
   </si>
@@ -602,9 +602,6 @@
     <t>SE 3250</t>
   </si>
   <si>
-    <t>Advanced Algorithms (Req MAT3310)</t>
-  </si>
-  <si>
     <t>Personal Software Practices</t>
   </si>
   <si>
@@ -624,6 +621,120 @@
   </si>
   <si>
     <t>SE 4400</t>
+  </si>
+  <si>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>Prerequisites</t>
+  </si>
+  <si>
+    <t>Yr1 - Fall</t>
+  </si>
+  <si>
+    <t>MATH</t>
+  </si>
+  <si>
+    <t>Calc I</t>
+  </si>
+  <si>
+    <t>ENGL</t>
+  </si>
+  <si>
+    <t>Composition</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>Life Science</t>
+  </si>
+  <si>
+    <t>Research Writing</t>
+  </si>
+  <si>
+    <t>ENGL 1010</t>
+  </si>
+  <si>
+    <t>Yr1 - Spring</t>
+  </si>
+  <si>
+    <t>Technical Communications</t>
+  </si>
+  <si>
+    <t>ENGL 2010</t>
+  </si>
+  <si>
+    <t>Yr3 - Spring</t>
+  </si>
+  <si>
+    <t>Calc II</t>
+  </si>
+  <si>
+    <t>MATH 1210</t>
+  </si>
+  <si>
+    <t>American Institutions</t>
+  </si>
+  <si>
+    <t>Yr2 - Fall</t>
+  </si>
+  <si>
+    <t>Discrete</t>
+  </si>
+  <si>
+    <t>Linear Algebra</t>
+  </si>
+  <si>
+    <t>PHYS</t>
+  </si>
+  <si>
+    <t>Physics for Science &amp; Engineers I</t>
+  </si>
+  <si>
+    <t>Physics Lab</t>
+  </si>
+  <si>
+    <t>FA/HU/SS</t>
+  </si>
+  <si>
+    <t>Yr2 - Spring</t>
+  </si>
+  <si>
+    <t>MAT/SCI</t>
+  </si>
+  <si>
+    <t>Elective</t>
+  </si>
+  <si>
+    <t>Physics for Science &amp; Engineers II</t>
+  </si>
+  <si>
+    <t>PHYS 2210</t>
+  </si>
+  <si>
+    <t>Yr3 - Fall</t>
+  </si>
+  <si>
+    <t>Stats for Science &amp; Engineers</t>
+  </si>
+  <si>
+    <t>Yr4 - Fall</t>
+  </si>
+  <si>
+    <t>Yr4 - Spring</t>
+  </si>
+  <si>
+    <t>COMM</t>
+  </si>
+  <si>
+    <t>Communications (?)</t>
+  </si>
+  <si>
+    <t>MATH 3310</t>
+  </si>
+  <si>
+    <t>Advanced Algorithms</t>
   </si>
 </sst>
 </file>
@@ -682,11 +793,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D61D163-DDAA-4B95-8176-F89699E1E41A}" name="Table1" displayName="Table1" ref="A1:D191" totalsRowShown="0">
-  <autoFilter ref="A1:D191" xr:uid="{1705DBE2-8C7E-4F78-90B2-A74D74893A95}"/>
-  <sortState ref="A2:D191">
-    <sortCondition ref="A2:A191"/>
-    <sortCondition ref="B2:B191"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D61D163-DDAA-4B95-8176-F89699E1E41A}" name="Table1" displayName="Table1" ref="A1:D262" totalsRowShown="0">
+  <autoFilter ref="A1:D262" xr:uid="{1705DBE2-8C7E-4F78-90B2-A74D74893A95}"/>
+  <sortState ref="A2:D262">
+    <sortCondition ref="A2:A262"/>
+    <sortCondition ref="B2:B262"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{5119BF1B-9C29-4FEB-AC7E-8AB780AA86D7}" name="Area"/>
@@ -995,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F90E087-F363-4783-84FA-5A2E6F319782}">
-  <dimension ref="A1:D191"/>
+  <dimension ref="A1:D262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="D177" sqref="D177"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1023,30 +1134,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>217</v>
       </c>
       <c r="B2">
-        <v>1400</v>
+        <v>1020</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>217</v>
       </c>
       <c r="B3">
-        <v>1400</v>
+        <v>1020</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1060,7 +1171,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1071,10 +1182,10 @@
         <v>1400</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1085,10 +1196,10 @@
         <v>1400</v>
       </c>
       <c r="C6" t="s">
-        <v>143</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>144</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1096,13 +1207,13 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>1410</v>
+        <v>1400</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1110,13 +1221,13 @@
         <v>2</v>
       </c>
       <c r="B8">
-        <v>1410</v>
+        <v>1400</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1124,13 +1235,13 @@
         <v>2</v>
       </c>
       <c r="B9">
-        <v>1410</v>
+        <v>1400</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>183</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1138,13 +1249,13 @@
         <v>2</v>
       </c>
       <c r="B10">
-        <v>1410</v>
+        <v>1405</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1155,10 +1266,10 @@
         <v>1410</v>
       </c>
       <c r="C11" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1169,10 +1280,10 @@
         <v>1410</v>
       </c>
       <c r="C12" t="s">
-        <v>148</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>149</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1180,13 +1291,13 @@
         <v>2</v>
       </c>
       <c r="B13">
-        <v>1810</v>
+        <v>1410</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1194,13 +1305,13 @@
         <v>2</v>
       </c>
       <c r="B14">
-        <v>1810</v>
+        <v>1410</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1208,13 +1319,13 @@
         <v>2</v>
       </c>
       <c r="B15">
-        <v>1810</v>
+        <v>1410</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1222,13 +1333,13 @@
         <v>2</v>
       </c>
       <c r="B16">
-        <v>1810</v>
+        <v>1410</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>148</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1236,13 +1347,13 @@
         <v>2</v>
       </c>
       <c r="B17">
-        <v>1810</v>
+        <v>1410</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1250,13 +1361,13 @@
         <v>2</v>
       </c>
       <c r="B18">
-        <v>1810</v>
+        <v>1415</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1270,7 +1381,7 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1284,7 +1395,7 @@
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1298,7 +1409,7 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1312,7 +1423,7 @@
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1326,7 +1437,7 @@
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1340,7 +1451,7 @@
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1351,10 +1462,10 @@
         <v>1810</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1365,10 +1476,10 @@
         <v>1810</v>
       </c>
       <c r="C26" t="s">
-        <v>143</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>150</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1379,10 +1490,10 @@
         <v>1810</v>
       </c>
       <c r="C27" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>151</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1390,13 +1501,13 @@
         <v>2</v>
       </c>
       <c r="B28">
-        <v>1820</v>
+        <v>1810</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1404,13 +1515,13 @@
         <v>2</v>
       </c>
       <c r="B29">
-        <v>1820</v>
+        <v>1810</v>
       </c>
       <c r="C29" t="s">
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1418,13 +1529,13 @@
         <v>2</v>
       </c>
       <c r="B30">
-        <v>1820</v>
+        <v>1810</v>
       </c>
       <c r="C30" t="s">
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1432,13 +1543,13 @@
         <v>2</v>
       </c>
       <c r="B31">
-        <v>1820</v>
+        <v>1810</v>
       </c>
       <c r="C31" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1446,13 +1557,13 @@
         <v>2</v>
       </c>
       <c r="B32">
-        <v>1820</v>
+        <v>1810</v>
       </c>
       <c r="C32" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1460,13 +1571,13 @@
         <v>2</v>
       </c>
       <c r="B33">
-        <v>1820</v>
+        <v>1810</v>
       </c>
       <c r="C33" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D33" t="s">
-        <v>32</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1474,13 +1585,13 @@
         <v>2</v>
       </c>
       <c r="B34">
-        <v>1820</v>
+        <v>1810</v>
       </c>
       <c r="C34" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1494,7 +1605,7 @@
         <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1505,10 +1616,10 @@
         <v>1820</v>
       </c>
       <c r="C36" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1519,10 +1630,10 @@
         <v>1820</v>
       </c>
       <c r="C37" t="s">
-        <v>143</v>
+        <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>152</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1533,10 +1644,10 @@
         <v>1820</v>
       </c>
       <c r="C38" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>153</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1544,13 +1655,13 @@
         <v>2</v>
       </c>
       <c r="B39">
-        <v>2420</v>
+        <v>1820</v>
       </c>
       <c r="C39" t="s">
         <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1558,13 +1669,13 @@
         <v>2</v>
       </c>
       <c r="B40">
-        <v>2420</v>
+        <v>1820</v>
       </c>
       <c r="C40" t="s">
         <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1572,13 +1683,13 @@
         <v>2</v>
       </c>
       <c r="B41">
-        <v>2420</v>
+        <v>1820</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1586,13 +1697,13 @@
         <v>2</v>
       </c>
       <c r="B42">
-        <v>2420</v>
+        <v>1820</v>
       </c>
       <c r="C42" t="s">
         <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1600,13 +1711,13 @@
         <v>2</v>
       </c>
       <c r="B43">
-        <v>2420</v>
+        <v>1820</v>
       </c>
       <c r="C43" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1614,13 +1725,13 @@
         <v>2</v>
       </c>
       <c r="B44">
-        <v>2420</v>
+        <v>1820</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="D44" t="s">
-        <v>38</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1628,13 +1739,13 @@
         <v>2</v>
       </c>
       <c r="B45">
-        <v>2420</v>
+        <v>1820</v>
       </c>
       <c r="C45" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D45" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1642,13 +1753,13 @@
         <v>2</v>
       </c>
       <c r="B46">
-        <v>2420</v>
+        <v>1820</v>
       </c>
       <c r="C46" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="D46" t="s">
-        <v>151</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1656,13 +1767,13 @@
         <v>2</v>
       </c>
       <c r="B47">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C47" t="s">
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1670,13 +1781,13 @@
         <v>2</v>
       </c>
       <c r="B48">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C48" t="s">
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1684,13 +1795,13 @@
         <v>2</v>
       </c>
       <c r="B49">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C49" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1698,13 +1809,13 @@
         <v>2</v>
       </c>
       <c r="B50">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C50" t="s">
         <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1712,13 +1823,13 @@
         <v>2</v>
       </c>
       <c r="B51">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C51" t="s">
         <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1726,13 +1837,13 @@
         <v>2</v>
       </c>
       <c r="B52">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C52" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1740,13 +1851,13 @@
         <v>2</v>
       </c>
       <c r="B53">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C53" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D53" t="s">
-        <v>45</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1754,13 +1865,13 @@
         <v>2</v>
       </c>
       <c r="B54">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C54" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D54" t="s">
-        <v>46</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1768,13 +1879,13 @@
         <v>2</v>
       </c>
       <c r="B55">
-        <v>2450</v>
+        <v>2420</v>
       </c>
       <c r="C55" t="s">
-        <v>10</v>
+        <v>183</v>
       </c>
       <c r="D55" t="s">
-        <v>47</v>
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1785,10 +1896,10 @@
         <v>2450</v>
       </c>
       <c r="C56" t="s">
-        <v>143</v>
+        <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>154</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1799,10 +1910,10 @@
         <v>2450</v>
       </c>
       <c r="C57" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>155</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1810,13 +1921,13 @@
         <v>2</v>
       </c>
       <c r="B58">
-        <v>2810</v>
+        <v>2450</v>
       </c>
       <c r="C58" t="s">
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1824,13 +1935,13 @@
         <v>2</v>
       </c>
       <c r="B59">
-        <v>2810</v>
+        <v>2450</v>
       </c>
       <c r="C59" t="s">
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1838,13 +1949,13 @@
         <v>2</v>
       </c>
       <c r="B60">
-        <v>2810</v>
+        <v>2450</v>
       </c>
       <c r="C60" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1852,13 +1963,13 @@
         <v>2</v>
       </c>
       <c r="B61">
-        <v>2810</v>
+        <v>2450</v>
       </c>
       <c r="C61" t="s">
-        <v>143</v>
+        <v>3</v>
       </c>
       <c r="D61" t="s">
-        <v>157</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1866,13 +1977,13 @@
         <v>2</v>
       </c>
       <c r="B62">
-        <v>2810</v>
+        <v>2450</v>
       </c>
       <c r="C62" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="D62" t="s">
-        <v>155</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1880,13 +1991,13 @@
         <v>2</v>
       </c>
       <c r="B63">
-        <v>2830</v>
+        <v>2450</v>
       </c>
       <c r="C63" t="s">
         <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1894,13 +2005,13 @@
         <v>2</v>
       </c>
       <c r="B64">
-        <v>2830</v>
+        <v>2450</v>
       </c>
       <c r="C64" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D64" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1908,13 +2019,13 @@
         <v>2</v>
       </c>
       <c r="B65">
-        <v>2830</v>
+        <v>2450</v>
       </c>
       <c r="C65" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D65" t="s">
-        <v>53</v>
+        <v>154</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1922,13 +2033,13 @@
         <v>2</v>
       </c>
       <c r="B66">
-        <v>2830</v>
+        <v>2450</v>
       </c>
       <c r="C66" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D66" t="s">
-        <v>54</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1936,13 +2047,13 @@
         <v>2</v>
       </c>
       <c r="B67">
-        <v>2830</v>
+        <v>2450</v>
       </c>
       <c r="C67" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D67" t="s">
-        <v>55</v>
+        <v>208</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1950,13 +2061,13 @@
         <v>2</v>
       </c>
       <c r="B68">
-        <v>2830</v>
+        <v>2700</v>
       </c>
       <c r="C68" t="s">
-        <v>10</v>
+        <v>183</v>
       </c>
       <c r="D68" t="s">
-        <v>56</v>
+        <v>194</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1964,13 +2075,13 @@
         <v>2</v>
       </c>
       <c r="B69">
-        <v>2830</v>
+        <v>2810</v>
       </c>
       <c r="C69" t="s">
-        <v>143</v>
+        <v>3</v>
       </c>
       <c r="D69" t="s">
-        <v>158</v>
+        <v>48</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1978,13 +2089,13 @@
         <v>2</v>
       </c>
       <c r="B70">
-        <v>2830</v>
+        <v>2810</v>
       </c>
       <c r="C70" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="D70" t="s">
-        <v>159</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1992,13 +2103,13 @@
         <v>2</v>
       </c>
       <c r="B71">
-        <v>2860</v>
+        <v>2810</v>
       </c>
       <c r="C71" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D71" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -2006,13 +2117,13 @@
         <v>2</v>
       </c>
       <c r="B72">
-        <v>2860</v>
+        <v>2810</v>
       </c>
       <c r="C72" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D72" t="s">
-        <v>58</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -2020,13 +2131,13 @@
         <v>2</v>
       </c>
       <c r="B73">
-        <v>2860</v>
+        <v>2810</v>
       </c>
       <c r="C73" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D73" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -2034,13 +2145,13 @@
         <v>2</v>
       </c>
       <c r="B74">
-        <v>2860</v>
+        <v>2810</v>
       </c>
       <c r="C74" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D74" t="s">
-        <v>60</v>
+        <v>201</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -2048,13 +2159,13 @@
         <v>2</v>
       </c>
       <c r="B75">
-        <v>2860</v>
+        <v>2830</v>
       </c>
       <c r="C75" t="s">
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -2062,13 +2173,13 @@
         <v>2</v>
       </c>
       <c r="B76">
-        <v>2860</v>
+        <v>2830</v>
       </c>
       <c r="C76" t="s">
         <v>3</v>
       </c>
       <c r="D76" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -2076,13 +2187,13 @@
         <v>2</v>
       </c>
       <c r="B77">
-        <v>2860</v>
+        <v>2830</v>
       </c>
       <c r="C77" t="s">
         <v>3</v>
       </c>
       <c r="D77" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -2090,13 +2201,13 @@
         <v>2</v>
       </c>
       <c r="B78">
-        <v>2860</v>
+        <v>2830</v>
       </c>
       <c r="C78" t="s">
         <v>3</v>
       </c>
       <c r="D78" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -2104,13 +2215,13 @@
         <v>2</v>
       </c>
       <c r="B79">
-        <v>2860</v>
+        <v>2830</v>
       </c>
       <c r="C79" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -2118,13 +2229,13 @@
         <v>2</v>
       </c>
       <c r="B80">
-        <v>2860</v>
+        <v>2830</v>
       </c>
       <c r="C80" t="s">
-        <v>143</v>
+        <v>10</v>
       </c>
       <c r="D80" t="s">
-        <v>160</v>
+        <v>56</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -2132,13 +2243,13 @@
         <v>2</v>
       </c>
       <c r="B81">
-        <v>2860</v>
+        <v>2830</v>
       </c>
       <c r="C81" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D81" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -2146,13 +2257,13 @@
         <v>2</v>
       </c>
       <c r="B82">
-        <v>3250</v>
+        <v>2830</v>
       </c>
       <c r="C82" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D82" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -2160,769 +2271,769 @@
         <v>2</v>
       </c>
       <c r="B83">
-        <v>3250</v>
+        <v>2830</v>
       </c>
       <c r="C83" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="D83" t="s">
-        <v>155</v>
+        <v>215</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B84">
-        <v>3250</v>
+        <v>2860</v>
       </c>
       <c r="C84" t="s">
         <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B85">
-        <v>3250</v>
+        <v>2860</v>
       </c>
       <c r="C85" t="s">
         <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B86">
-        <v>3250</v>
+        <v>2860</v>
       </c>
       <c r="C86" t="s">
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B87">
-        <v>3250</v>
+        <v>2860</v>
       </c>
       <c r="C87" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D87" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B88">
-        <v>3410</v>
+        <v>2860</v>
       </c>
       <c r="C88" t="s">
         <v>3</v>
       </c>
       <c r="D88" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B89">
-        <v>3410</v>
+        <v>2860</v>
       </c>
       <c r="C89" t="s">
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B90">
-        <v>3410</v>
+        <v>2860</v>
       </c>
       <c r="C90" t="s">
         <v>3</v>
       </c>
       <c r="D90" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B91">
-        <v>3410</v>
+        <v>2860</v>
       </c>
       <c r="C91" t="s">
         <v>3</v>
       </c>
       <c r="D91" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B92">
-        <v>3410</v>
+        <v>2860</v>
       </c>
       <c r="C92" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D92" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B93">
-        <v>3410</v>
+        <v>2860</v>
       </c>
       <c r="C93" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D93" t="s">
-        <v>76</v>
+        <v>160</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B94">
-        <v>3410</v>
+        <v>2860</v>
       </c>
       <c r="C94" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D94" t="s">
-        <v>77</v>
+        <v>161</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="B95">
-        <v>3410</v>
+        <v>2860</v>
       </c>
       <c r="C95" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D95" t="s">
-        <v>78</v>
+        <v>208</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>66</v>
+        <v>188</v>
       </c>
       <c r="B96">
-        <v>3410</v>
+        <v>1010</v>
       </c>
       <c r="C96" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D96" t="s">
-        <v>79</v>
+        <v>189</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>66</v>
+        <v>188</v>
       </c>
       <c r="B97">
-        <v>3410</v>
+        <v>1010</v>
       </c>
       <c r="C97" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D97" t="s">
-        <v>80</v>
+        <v>185</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>66</v>
+        <v>188</v>
       </c>
       <c r="B98">
-        <v>3410</v>
+        <v>2010</v>
       </c>
       <c r="C98" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="D98" t="s">
-        <v>81</v>
+        <v>192</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>66</v>
+        <v>188</v>
       </c>
       <c r="B99">
-        <v>3410</v>
+        <v>2010</v>
       </c>
       <c r="C99" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D99" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>66</v>
+        <v>188</v>
       </c>
       <c r="B100">
-        <v>3410</v>
+        <v>2010</v>
       </c>
       <c r="C100" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="D100" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>66</v>
+        <v>188</v>
       </c>
       <c r="B101">
-        <v>3450</v>
+        <v>3260</v>
       </c>
       <c r="C101" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D101" t="s">
-        <v>82</v>
+        <v>195</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>66</v>
+        <v>188</v>
       </c>
       <c r="B102">
-        <v>3450</v>
+        <v>3260</v>
       </c>
       <c r="C102" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D102" t="s">
-        <v>83</v>
+        <v>196</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>66</v>
+        <v>188</v>
       </c>
       <c r="B103">
-        <v>3450</v>
+        <v>3260</v>
       </c>
       <c r="C103" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D103" t="s">
-        <v>84</v>
+        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="B104">
-        <v>3450</v>
+        <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="D104" t="s">
-        <v>85</v>
+        <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="B105">
-        <v>3450</v>
+        <v>2</v>
       </c>
       <c r="C105" t="s">
         <v>143</v>
       </c>
       <c r="D105" t="s">
-        <v>165</v>
+        <v>200</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="B106">
-        <v>3450</v>
+        <v>2</v>
       </c>
       <c r="C106" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="D106" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="B107">
-        <v>3520</v>
+        <v>3</v>
       </c>
       <c r="C107" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D107" t="s">
-        <v>86</v>
+        <v>207</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="B108">
-        <v>3520</v>
+        <v>3</v>
       </c>
       <c r="C108" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D108" t="s">
-        <v>87</v>
+        <v>201</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="B109">
-        <v>3520</v>
+        <v>4</v>
       </c>
       <c r="C109" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D109" t="s">
-        <v>88</v>
+        <v>207</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="B110">
-        <v>3520</v>
+        <v>4</v>
       </c>
       <c r="C110" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D110" t="s">
-        <v>89</v>
+        <v>208</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="B111">
-        <v>3520</v>
+        <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D111" t="s">
-        <v>90</v>
+        <v>207</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="B112">
-        <v>3520</v>
+        <v>5</v>
       </c>
       <c r="C112" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D112" t="s">
-        <v>91</v>
+        <v>197</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>66</v>
+        <v>209</v>
       </c>
       <c r="B113">
-        <v>3520</v>
+        <v>1</v>
       </c>
       <c r="C113" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D113" t="s">
-        <v>92</v>
+        <v>210</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>66</v>
+        <v>209</v>
       </c>
       <c r="B114">
-        <v>3520</v>
+        <v>1</v>
       </c>
       <c r="C114" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D114" t="s">
-        <v>93</v>
+        <v>208</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="B115">
-        <v>3520</v>
+        <v>1210</v>
       </c>
       <c r="C115" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="D115" t="s">
-        <v>94</v>
+        <v>187</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="B116">
-        <v>3520</v>
+        <v>1210</v>
       </c>
       <c r="C116" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="D116" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="B117">
-        <v>3520</v>
+        <v>1210</v>
       </c>
       <c r="C117" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D117" t="s">
-        <v>155</v>
+        <v>198</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="B118">
-        <v>3620</v>
+        <v>1220</v>
       </c>
       <c r="C118" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D118" t="s">
-        <v>95</v>
+        <v>199</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="B119">
-        <v>3620</v>
+        <v>1220</v>
       </c>
       <c r="C119" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D119" t="s">
-        <v>96</v>
+        <v>194</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="B120">
-        <v>3620</v>
+        <v>2270</v>
       </c>
       <c r="C120" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D120" t="s">
-        <v>97</v>
+        <v>203</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="B121">
-        <v>3620</v>
+        <v>2270</v>
       </c>
       <c r="C121" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D121" t="s">
-        <v>98</v>
+        <v>199</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="B122">
-        <v>3620</v>
+        <v>2270</v>
       </c>
       <c r="C122" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D122" t="s">
-        <v>99</v>
+        <v>201</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="B123">
-        <v>3620</v>
+        <v>3040</v>
       </c>
       <c r="C123" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="D123" t="s">
-        <v>100</v>
+        <v>214</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="B124">
-        <v>3620</v>
+        <v>3040</v>
       </c>
       <c r="C124" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D124" t="s">
-        <v>167</v>
+        <v>199</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="B125">
-        <v>3620</v>
+        <v>3040</v>
       </c>
       <c r="C125" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="D125" t="s">
-        <v>168</v>
+        <v>213</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="B126">
-        <v>3620</v>
+        <v>3310</v>
       </c>
       <c r="C126" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D126" t="s">
-        <v>169</v>
+        <v>202</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="B127">
-        <v>3630</v>
+        <v>3310</v>
       </c>
       <c r="C127" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D127" t="s">
-        <v>101</v>
+        <v>199</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="B128">
-        <v>3630</v>
+        <v>3310</v>
       </c>
       <c r="C128" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D128" t="s">
-        <v>102</v>
+        <v>201</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>66</v>
+        <v>204</v>
       </c>
       <c r="B129">
-        <v>3630</v>
+        <v>2210</v>
       </c>
       <c r="C129" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="D129" t="s">
-        <v>103</v>
+        <v>205</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>66</v>
+        <v>204</v>
       </c>
       <c r="B130">
-        <v>3630</v>
+        <v>2210</v>
       </c>
       <c r="C130" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="D130" t="s">
-        <v>170</v>
+        <v>201</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>66</v>
+        <v>204</v>
       </c>
       <c r="B131">
-        <v>3630</v>
+        <v>2215</v>
       </c>
       <c r="C131" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D131" t="s">
-        <v>155</v>
+        <v>206</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>66</v>
+        <v>204</v>
       </c>
       <c r="B132">
-        <v>4120</v>
+        <v>2215</v>
       </c>
       <c r="C132" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D132" t="s">
-        <v>104</v>
+        <v>201</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>66</v>
+        <v>204</v>
       </c>
       <c r="B133">
-        <v>4120</v>
+        <v>2220</v>
       </c>
       <c r="C133" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D133" t="s">
-        <v>105</v>
+        <v>211</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>66</v>
+        <v>204</v>
       </c>
       <c r="B134">
-        <v>4120</v>
+        <v>2220</v>
       </c>
       <c r="C134" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D134" t="s">
-        <v>106</v>
+        <v>212</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>66</v>
+        <v>204</v>
       </c>
       <c r="B135">
-        <v>4120</v>
+        <v>2220</v>
       </c>
       <c r="C135" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D135" t="s">
-        <v>107</v>
+        <v>208</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>66</v>
+        <v>204</v>
       </c>
       <c r="B136">
-        <v>4120</v>
+        <v>2225</v>
       </c>
       <c r="C136" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D136" t="s">
-        <v>108</v>
+        <v>206</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>66</v>
+        <v>204</v>
       </c>
       <c r="B137">
-        <v>4120</v>
+        <v>2225</v>
       </c>
       <c r="C137" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D137" t="s">
-        <v>109</v>
+        <v>208</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
@@ -2930,13 +3041,13 @@
         <v>66</v>
       </c>
       <c r="B138">
-        <v>4120</v>
+        <v>3250</v>
       </c>
       <c r="C138" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="D138" t="s">
-        <v>110</v>
+        <v>162</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
@@ -2944,13 +3055,13 @@
         <v>66</v>
       </c>
       <c r="B139">
-        <v>4120</v>
+        <v>3250</v>
       </c>
       <c r="C139" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D139" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
@@ -2958,13 +3069,13 @@
         <v>66</v>
       </c>
       <c r="B140">
-        <v>4120</v>
+        <v>3250</v>
       </c>
       <c r="C140" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="D140" t="s">
-        <v>172</v>
+        <v>67</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
@@ -2972,13 +3083,13 @@
         <v>66</v>
       </c>
       <c r="B141">
-        <v>4140</v>
+        <v>3250</v>
       </c>
       <c r="C141" t="s">
         <v>3</v>
       </c>
       <c r="D141" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
@@ -2986,13 +3097,13 @@
         <v>66</v>
       </c>
       <c r="B142">
-        <v>4140</v>
+        <v>3250</v>
       </c>
       <c r="C142" t="s">
         <v>3</v>
       </c>
       <c r="D142" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
@@ -3000,13 +3111,13 @@
         <v>66</v>
       </c>
       <c r="B143">
-        <v>4140</v>
+        <v>3250</v>
       </c>
       <c r="C143" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D143" t="s">
-        <v>113</v>
+        <v>70</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
@@ -3014,13 +3125,13 @@
         <v>66</v>
       </c>
       <c r="B144">
-        <v>4140</v>
+        <v>3250</v>
       </c>
       <c r="C144" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D144" t="s">
-        <v>114</v>
+        <v>213</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
@@ -3028,13 +3139,13 @@
         <v>66</v>
       </c>
       <c r="B145">
-        <v>4140</v>
+        <v>3410</v>
       </c>
       <c r="C145" t="s">
         <v>3</v>
       </c>
       <c r="D145" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
@@ -3042,27 +3153,27 @@
         <v>66</v>
       </c>
       <c r="B146">
-        <v>4140</v>
+        <v>3410</v>
       </c>
       <c r="C146" t="s">
         <v>3</v>
       </c>
       <c r="D146" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>66</v>
       </c>
       <c r="B147">
-        <v>4140</v>
+        <v>3410</v>
       </c>
       <c r="C147" t="s">
-        <v>10</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>117</v>
+        <v>3</v>
+      </c>
+      <c r="D147" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
@@ -3070,13 +3181,13 @@
         <v>66</v>
       </c>
       <c r="B148">
-        <v>4140</v>
+        <v>3410</v>
       </c>
       <c r="C148" t="s">
-        <v>143</v>
+        <v>3</v>
       </c>
       <c r="D148" t="s">
-        <v>173</v>
+        <v>74</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
@@ -3084,13 +3195,13 @@
         <v>66</v>
       </c>
       <c r="B149">
-        <v>4140</v>
+        <v>3410</v>
       </c>
       <c r="C149" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="D149" t="s">
-        <v>172</v>
+        <v>75</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
@@ -3098,13 +3209,13 @@
         <v>66</v>
       </c>
       <c r="B150">
-        <v>4220</v>
+        <v>3410</v>
       </c>
       <c r="C150" t="s">
         <v>3</v>
       </c>
       <c r="D150" t="s">
-        <v>118</v>
+        <v>76</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
@@ -3112,13 +3223,13 @@
         <v>66</v>
       </c>
       <c r="B151">
-        <v>4220</v>
+        <v>3410</v>
       </c>
       <c r="C151" t="s">
         <v>3</v>
       </c>
       <c r="D151" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
@@ -3126,27 +3237,27 @@
         <v>66</v>
       </c>
       <c r="B152">
-        <v>4220</v>
+        <v>3410</v>
       </c>
       <c r="C152" t="s">
         <v>3</v>
       </c>
       <c r="D152" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" ht="302.39999999999998" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>66</v>
       </c>
       <c r="B153">
-        <v>4220</v>
+        <v>3410</v>
       </c>
       <c r="C153" t="s">
-        <v>10</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>121</v>
+        <v>3</v>
+      </c>
+      <c r="D153" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
@@ -3154,13 +3265,13 @@
         <v>66</v>
       </c>
       <c r="B154">
-        <v>4220</v>
+        <v>3410</v>
       </c>
       <c r="C154" t="s">
-        <v>143</v>
+        <v>3</v>
       </c>
       <c r="D154" t="s">
-        <v>174</v>
+        <v>80</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
@@ -3168,13 +3279,13 @@
         <v>66</v>
       </c>
       <c r="B155">
-        <v>4220</v>
+        <v>3410</v>
       </c>
       <c r="C155" t="s">
-        <v>145</v>
+        <v>10</v>
       </c>
       <c r="D155" t="s">
-        <v>175</v>
+        <v>81</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
@@ -3182,13 +3293,13 @@
         <v>66</v>
       </c>
       <c r="B156">
-        <v>4220</v>
+        <v>3410</v>
       </c>
       <c r="C156" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D156" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
@@ -3196,13 +3307,13 @@
         <v>66</v>
       </c>
       <c r="B157">
-        <v>4230</v>
+        <v>3410</v>
       </c>
       <c r="C157" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D157" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
@@ -3210,13 +3321,13 @@
         <v>66</v>
       </c>
       <c r="B158">
-        <v>4230</v>
+        <v>3410</v>
       </c>
       <c r="C158" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D158" t="s">
-        <v>123</v>
+        <v>213</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
@@ -3224,13 +3335,13 @@
         <v>66</v>
       </c>
       <c r="B159">
-        <v>4230</v>
+        <v>3450</v>
       </c>
       <c r="C159" t="s">
         <v>3</v>
       </c>
       <c r="D159" t="s">
-        <v>124</v>
+        <v>82</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
@@ -3238,13 +3349,13 @@
         <v>66</v>
       </c>
       <c r="B160">
-        <v>4230</v>
+        <v>3450</v>
       </c>
       <c r="C160" t="s">
         <v>3</v>
       </c>
       <c r="D160" t="s">
-        <v>125</v>
+        <v>83</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
@@ -3252,13 +3363,13 @@
         <v>66</v>
       </c>
       <c r="B161">
-        <v>4230</v>
+        <v>3450</v>
       </c>
       <c r="C161" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D161" t="s">
-        <v>126</v>
+        <v>84</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
@@ -3266,13 +3377,13 @@
         <v>66</v>
       </c>
       <c r="B162">
-        <v>4230</v>
+        <v>3450</v>
       </c>
       <c r="C162" t="s">
-        <v>143</v>
+        <v>10</v>
       </c>
       <c r="D162" t="s">
-        <v>176</v>
+        <v>85</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
@@ -3280,13 +3391,13 @@
         <v>66</v>
       </c>
       <c r="B163">
-        <v>4230</v>
+        <v>3450</v>
       </c>
       <c r="C163" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D163" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
@@ -3294,13 +3405,13 @@
         <v>66</v>
       </c>
       <c r="B164">
-        <v>4320</v>
+        <v>3450</v>
       </c>
       <c r="C164" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D164" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
@@ -3308,13 +3419,13 @@
         <v>66</v>
       </c>
       <c r="B165">
-        <v>4320</v>
+        <v>3450</v>
       </c>
       <c r="C165" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D165" t="s">
-        <v>128</v>
+        <v>197</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
@@ -3322,13 +3433,13 @@
         <v>66</v>
       </c>
       <c r="B166">
-        <v>4320</v>
+        <v>3520</v>
       </c>
       <c r="C166" t="s">
         <v>3</v>
       </c>
       <c r="D166" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
@@ -3336,27 +3447,27 @@
         <v>66</v>
       </c>
       <c r="B167">
-        <v>4320</v>
+        <v>3520</v>
       </c>
       <c r="C167" t="s">
         <v>3</v>
       </c>
       <c r="D167" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>66</v>
       </c>
       <c r="B168">
-        <v>4320</v>
+        <v>3520</v>
       </c>
       <c r="C168" t="s">
-        <v>10</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>131</v>
+        <v>3</v>
+      </c>
+      <c r="D168" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
@@ -3364,13 +3475,13 @@
         <v>66</v>
       </c>
       <c r="B169">
-        <v>4320</v>
+        <v>3520</v>
       </c>
       <c r="C169" t="s">
-        <v>143</v>
+        <v>3</v>
       </c>
       <c r="D169" t="s">
-        <v>177</v>
+        <v>89</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
@@ -3378,13 +3489,13 @@
         <v>66</v>
       </c>
       <c r="B170">
-        <v>4320</v>
+        <v>3520</v>
       </c>
       <c r="C170" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="D170" t="s">
-        <v>178</v>
+        <v>90</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
@@ -3392,13 +3503,13 @@
         <v>66</v>
       </c>
       <c r="B171">
-        <v>4340</v>
+        <v>3520</v>
       </c>
       <c r="C171" t="s">
         <v>3</v>
       </c>
       <c r="D171" t="s">
-        <v>132</v>
+        <v>91</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
@@ -3406,13 +3517,13 @@
         <v>66</v>
       </c>
       <c r="B172">
-        <v>4340</v>
+        <v>3520</v>
       </c>
       <c r="C172" t="s">
         <v>3</v>
       </c>
       <c r="D172" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
@@ -3420,13 +3531,13 @@
         <v>66</v>
       </c>
       <c r="B173">
-        <v>4340</v>
+        <v>3520</v>
       </c>
       <c r="C173" t="s">
         <v>3</v>
       </c>
       <c r="D173" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
@@ -3434,13 +3545,13 @@
         <v>66</v>
       </c>
       <c r="B174">
-        <v>4340</v>
+        <v>3520</v>
       </c>
       <c r="C174" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D174" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
@@ -3448,27 +3559,27 @@
         <v>66</v>
       </c>
       <c r="B175">
-        <v>4340</v>
+        <v>3520</v>
       </c>
       <c r="C175" t="s">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="D175" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>66</v>
       </c>
       <c r="B176">
-        <v>4340</v>
+        <v>3520</v>
       </c>
       <c r="C176" t="s">
-        <v>10</v>
-      </c>
-      <c r="D176" s="1" t="s">
-        <v>137</v>
+        <v>145</v>
+      </c>
+      <c r="D176" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
@@ -3476,13 +3587,13 @@
         <v>66</v>
       </c>
       <c r="B177">
-        <v>4340</v>
+        <v>3520</v>
       </c>
       <c r="C177" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="D177" t="s">
-        <v>179</v>
+        <v>213</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
@@ -3490,13 +3601,13 @@
         <v>66</v>
       </c>
       <c r="B178">
-        <v>4340</v>
+        <v>3620</v>
       </c>
       <c r="C178" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="D178" t="s">
-        <v>180</v>
+        <v>95</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
@@ -3504,13 +3615,13 @@
         <v>66</v>
       </c>
       <c r="B179">
-        <v>4400</v>
+        <v>3620</v>
       </c>
       <c r="C179" t="s">
         <v>3</v>
       </c>
       <c r="D179" t="s">
-        <v>138</v>
+        <v>96</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
@@ -3518,13 +3629,13 @@
         <v>66</v>
       </c>
       <c r="B180">
-        <v>4400</v>
+        <v>3620</v>
       </c>
       <c r="C180" t="s">
         <v>3</v>
       </c>
       <c r="D180" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
@@ -3532,13 +3643,13 @@
         <v>66</v>
       </c>
       <c r="B181">
-        <v>4400</v>
+        <v>3620</v>
       </c>
       <c r="C181" t="s">
         <v>3</v>
       </c>
       <c r="D181" t="s">
-        <v>140</v>
+        <v>98</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
@@ -3546,13 +3657,13 @@
         <v>66</v>
       </c>
       <c r="B182">
-        <v>4400</v>
+        <v>3620</v>
       </c>
       <c r="C182" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D182" t="s">
-        <v>141</v>
+        <v>99</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
@@ -3560,13 +3671,13 @@
         <v>66</v>
       </c>
       <c r="B183">
-        <v>4400</v>
+        <v>3620</v>
       </c>
       <c r="C183" t="s">
-        <v>143</v>
+        <v>10</v>
       </c>
       <c r="D183" t="s">
-        <v>181</v>
+        <v>100</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
@@ -3574,13 +3685,13 @@
         <v>66</v>
       </c>
       <c r="B184">
-        <v>4400</v>
+        <v>3620</v>
       </c>
       <c r="C184" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D184" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
@@ -3588,13 +3699,13 @@
         <v>66</v>
       </c>
       <c r="B185">
-        <v>4400</v>
+        <v>3620</v>
       </c>
       <c r="C185" t="s">
         <v>145</v>
       </c>
       <c r="D185" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
@@ -3602,13 +3713,13 @@
         <v>66</v>
       </c>
       <c r="B186">
-        <v>4450</v>
+        <v>3620</v>
       </c>
       <c r="C186" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="D186" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
@@ -3616,13 +3727,13 @@
         <v>66</v>
       </c>
       <c r="B187">
-        <v>4450</v>
+        <v>3620</v>
       </c>
       <c r="C187" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="D187" t="s">
-        <v>139</v>
+        <v>197</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
@@ -3630,13 +3741,13 @@
         <v>66</v>
       </c>
       <c r="B188">
-        <v>4450</v>
+        <v>3630</v>
       </c>
       <c r="C188" t="s">
         <v>3</v>
       </c>
       <c r="D188" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
@@ -3644,13 +3755,13 @@
         <v>66</v>
       </c>
       <c r="B189">
-        <v>4450</v>
+        <v>3630</v>
       </c>
       <c r="C189" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D189" t="s">
-        <v>141</v>
+        <v>102</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
@@ -3658,13 +3769,13 @@
         <v>66</v>
       </c>
       <c r="B190">
-        <v>4450</v>
+        <v>3630</v>
       </c>
       <c r="C190" t="s">
-        <v>143</v>
+        <v>10</v>
       </c>
       <c r="D190" t="s">
-        <v>182</v>
+        <v>103</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
@@ -3672,13 +3783,1007 @@
         <v>66</v>
       </c>
       <c r="B191">
+        <v>3630</v>
+      </c>
+      <c r="C191" t="s">
+        <v>143</v>
+      </c>
+      <c r="D191" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>66</v>
+      </c>
+      <c r="B192">
+        <v>3630</v>
+      </c>
+      <c r="C192" t="s">
+        <v>145</v>
+      </c>
+      <c r="D192" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>66</v>
+      </c>
+      <c r="B193">
+        <v>3630</v>
+      </c>
+      <c r="C193" t="s">
+        <v>183</v>
+      </c>
+      <c r="D193" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>66</v>
+      </c>
+      <c r="B194">
+        <v>4120</v>
+      </c>
+      <c r="C194" t="s">
+        <v>3</v>
+      </c>
+      <c r="D194" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>66</v>
+      </c>
+      <c r="B195">
+        <v>4120</v>
+      </c>
+      <c r="C195" t="s">
+        <v>3</v>
+      </c>
+      <c r="D195" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>66</v>
+      </c>
+      <c r="B196">
+        <v>4120</v>
+      </c>
+      <c r="C196" t="s">
+        <v>3</v>
+      </c>
+      <c r="D196" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>66</v>
+      </c>
+      <c r="B197">
+        <v>4120</v>
+      </c>
+      <c r="C197" t="s">
+        <v>3</v>
+      </c>
+      <c r="D197" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>66</v>
+      </c>
+      <c r="B198">
+        <v>4120</v>
+      </c>
+      <c r="C198" t="s">
+        <v>3</v>
+      </c>
+      <c r="D198" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>66</v>
+      </c>
+      <c r="B199">
+        <v>4120</v>
+      </c>
+      <c r="C199" t="s">
+        <v>3</v>
+      </c>
+      <c r="D199" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>66</v>
+      </c>
+      <c r="B200">
+        <v>4120</v>
+      </c>
+      <c r="C200" t="s">
+        <v>10</v>
+      </c>
+      <c r="D200" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>66</v>
+      </c>
+      <c r="B201">
+        <v>4120</v>
+      </c>
+      <c r="C201" t="s">
+        <v>143</v>
+      </c>
+      <c r="D201" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>66</v>
+      </c>
+      <c r="B202">
+        <v>4120</v>
+      </c>
+      <c r="C202" t="s">
+        <v>145</v>
+      </c>
+      <c r="D202" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>66</v>
+      </c>
+      <c r="B203">
+        <v>4120</v>
+      </c>
+      <c r="C203" t="s">
+        <v>183</v>
+      </c>
+      <c r="D203" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>66</v>
+      </c>
+      <c r="B204">
+        <v>4140</v>
+      </c>
+      <c r="C204" t="s">
+        <v>3</v>
+      </c>
+      <c r="D204" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>66</v>
+      </c>
+      <c r="B205">
+        <v>4140</v>
+      </c>
+      <c r="C205" t="s">
+        <v>3</v>
+      </c>
+      <c r="D205" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>66</v>
+      </c>
+      <c r="B206">
+        <v>4140</v>
+      </c>
+      <c r="C206" t="s">
+        <v>3</v>
+      </c>
+      <c r="D206" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>66</v>
+      </c>
+      <c r="B207">
+        <v>4140</v>
+      </c>
+      <c r="C207" t="s">
+        <v>3</v>
+      </c>
+      <c r="D207" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>66</v>
+      </c>
+      <c r="B208">
+        <v>4140</v>
+      </c>
+      <c r="C208" t="s">
+        <v>3</v>
+      </c>
+      <c r="D208" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>66</v>
+      </c>
+      <c r="B209">
+        <v>4140</v>
+      </c>
+      <c r="C209" t="s">
+        <v>3</v>
+      </c>
+      <c r="D209" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>66</v>
+      </c>
+      <c r="B210">
+        <v>4140</v>
+      </c>
+      <c r="C210" t="s">
+        <v>10</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>66</v>
+      </c>
+      <c r="B211">
+        <v>4140</v>
+      </c>
+      <c r="C211" t="s">
+        <v>143</v>
+      </c>
+      <c r="D211" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>66</v>
+      </c>
+      <c r="B212">
+        <v>4140</v>
+      </c>
+      <c r="C212" t="s">
+        <v>145</v>
+      </c>
+      <c r="D212" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>66</v>
+      </c>
+      <c r="B213">
+        <v>4140</v>
+      </c>
+      <c r="C213" t="s">
+        <v>183</v>
+      </c>
+      <c r="D213" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>66</v>
+      </c>
+      <c r="B214">
+        <v>4220</v>
+      </c>
+      <c r="C214" t="s">
+        <v>3</v>
+      </c>
+      <c r="D214" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>66</v>
+      </c>
+      <c r="B215">
+        <v>4220</v>
+      </c>
+      <c r="C215" t="s">
+        <v>3</v>
+      </c>
+      <c r="D215" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>66</v>
+      </c>
+      <c r="B216">
+        <v>4220</v>
+      </c>
+      <c r="C216" t="s">
+        <v>3</v>
+      </c>
+      <c r="D216" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>66</v>
+      </c>
+      <c r="B217">
+        <v>4220</v>
+      </c>
+      <c r="C217" t="s">
+        <v>10</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>66</v>
+      </c>
+      <c r="B218">
+        <v>4220</v>
+      </c>
+      <c r="C218" t="s">
+        <v>143</v>
+      </c>
+      <c r="D218" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>66</v>
+      </c>
+      <c r="B219">
+        <v>4220</v>
+      </c>
+      <c r="C219" t="s">
+        <v>145</v>
+      </c>
+      <c r="D219" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>66</v>
+      </c>
+      <c r="B220">
+        <v>4220</v>
+      </c>
+      <c r="C220" t="s">
+        <v>145</v>
+      </c>
+      <c r="D220" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>66</v>
+      </c>
+      <c r="B221">
+        <v>4220</v>
+      </c>
+      <c r="C221" t="s">
+        <v>183</v>
+      </c>
+      <c r="D221" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>66</v>
+      </c>
+      <c r="B222">
+        <v>4230</v>
+      </c>
+      <c r="C222" t="s">
+        <v>3</v>
+      </c>
+      <c r="D222" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>66</v>
+      </c>
+      <c r="B223">
+        <v>4230</v>
+      </c>
+      <c r="C223" t="s">
+        <v>3</v>
+      </c>
+      <c r="D223" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>66</v>
+      </c>
+      <c r="B224">
+        <v>4230</v>
+      </c>
+      <c r="C224" t="s">
+        <v>3</v>
+      </c>
+      <c r="D224" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>66</v>
+      </c>
+      <c r="B225">
+        <v>4230</v>
+      </c>
+      <c r="C225" t="s">
+        <v>3</v>
+      </c>
+      <c r="D225" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>66</v>
+      </c>
+      <c r="B226">
+        <v>4230</v>
+      </c>
+      <c r="C226" t="s">
+        <v>10</v>
+      </c>
+      <c r="D226" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>66</v>
+      </c>
+      <c r="B227">
+        <v>4230</v>
+      </c>
+      <c r="C227" t="s">
+        <v>143</v>
+      </c>
+      <c r="D227" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>66</v>
+      </c>
+      <c r="B228">
+        <v>4230</v>
+      </c>
+      <c r="C228" t="s">
+        <v>145</v>
+      </c>
+      <c r="D228" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>66</v>
+      </c>
+      <c r="B229">
+        <v>4230</v>
+      </c>
+      <c r="C229" t="s">
+        <v>145</v>
+      </c>
+      <c r="D229" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>66</v>
+      </c>
+      <c r="B230">
+        <v>4230</v>
+      </c>
+      <c r="C230" t="s">
+        <v>183</v>
+      </c>
+      <c r="D230" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>66</v>
+      </c>
+      <c r="B231">
+        <v>4320</v>
+      </c>
+      <c r="C231" t="s">
+        <v>3</v>
+      </c>
+      <c r="D231" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>66</v>
+      </c>
+      <c r="B232">
+        <v>4320</v>
+      </c>
+      <c r="C232" t="s">
+        <v>3</v>
+      </c>
+      <c r="D232" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>66</v>
+      </c>
+      <c r="B233">
+        <v>4320</v>
+      </c>
+      <c r="C233" t="s">
+        <v>3</v>
+      </c>
+      <c r="D233" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>66</v>
+      </c>
+      <c r="B234">
+        <v>4320</v>
+      </c>
+      <c r="C234" t="s">
+        <v>3</v>
+      </c>
+      <c r="D234" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>66</v>
+      </c>
+      <c r="B235">
+        <v>4320</v>
+      </c>
+      <c r="C235" t="s">
+        <v>10</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>66</v>
+      </c>
+      <c r="B236">
+        <v>4320</v>
+      </c>
+      <c r="C236" t="s">
+        <v>143</v>
+      </c>
+      <c r="D236" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>66</v>
+      </c>
+      <c r="B237">
+        <v>4320</v>
+      </c>
+      <c r="C237" t="s">
+        <v>145</v>
+      </c>
+      <c r="D237" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>66</v>
+      </c>
+      <c r="B238">
+        <v>4320</v>
+      </c>
+      <c r="C238" t="s">
+        <v>183</v>
+      </c>
+      <c r="D238" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
+        <v>66</v>
+      </c>
+      <c r="B239">
+        <v>4340</v>
+      </c>
+      <c r="C239" t="s">
+        <v>3</v>
+      </c>
+      <c r="D239" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>66</v>
+      </c>
+      <c r="B240">
+        <v>4340</v>
+      </c>
+      <c r="C240" t="s">
+        <v>3</v>
+      </c>
+      <c r="D240" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
+        <v>66</v>
+      </c>
+      <c r="B241">
+        <v>4340</v>
+      </c>
+      <c r="C241" t="s">
+        <v>3</v>
+      </c>
+      <c r="D241" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>66</v>
+      </c>
+      <c r="B242">
+        <v>4340</v>
+      </c>
+      <c r="C242" t="s">
+        <v>3</v>
+      </c>
+      <c r="D242" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>66</v>
+      </c>
+      <c r="B243">
+        <v>4340</v>
+      </c>
+      <c r="C243" t="s">
+        <v>3</v>
+      </c>
+      <c r="D243" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
+        <v>66</v>
+      </c>
+      <c r="B244">
+        <v>4340</v>
+      </c>
+      <c r="C244" t="s">
+        <v>10</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
+        <v>66</v>
+      </c>
+      <c r="B245">
+        <v>4340</v>
+      </c>
+      <c r="C245" t="s">
+        <v>143</v>
+      </c>
+      <c r="D245" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
+        <v>66</v>
+      </c>
+      <c r="B246">
+        <v>4340</v>
+      </c>
+      <c r="C246" t="s">
+        <v>145</v>
+      </c>
+      <c r="D246" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
+        <v>66</v>
+      </c>
+      <c r="B247">
+        <v>4340</v>
+      </c>
+      <c r="C247" t="s">
+        <v>183</v>
+      </c>
+      <c r="D247" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
+        <v>66</v>
+      </c>
+      <c r="B248">
+        <v>4400</v>
+      </c>
+      <c r="C248" t="s">
+        <v>3</v>
+      </c>
+      <c r="D248" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>66</v>
+      </c>
+      <c r="B249">
+        <v>4400</v>
+      </c>
+      <c r="C249" t="s">
+        <v>3</v>
+      </c>
+      <c r="D249" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
+        <v>66</v>
+      </c>
+      <c r="B250">
+        <v>4400</v>
+      </c>
+      <c r="C250" t="s">
+        <v>3</v>
+      </c>
+      <c r="D250" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A251" t="s">
+        <v>66</v>
+      </c>
+      <c r="B251">
+        <v>4400</v>
+      </c>
+      <c r="C251" t="s">
+        <v>10</v>
+      </c>
+      <c r="D251" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
+        <v>66</v>
+      </c>
+      <c r="B252">
+        <v>4400</v>
+      </c>
+      <c r="C252" t="s">
+        <v>143</v>
+      </c>
+      <c r="D252" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A253" t="s">
+        <v>66</v>
+      </c>
+      <c r="B253">
+        <v>4400</v>
+      </c>
+      <c r="C253" t="s">
+        <v>145</v>
+      </c>
+      <c r="D253" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A254" t="s">
+        <v>66</v>
+      </c>
+      <c r="B254">
+        <v>4400</v>
+      </c>
+      <c r="C254" t="s">
+        <v>145</v>
+      </c>
+      <c r="D254" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
+        <v>66</v>
+      </c>
+      <c r="B255">
+        <v>4400</v>
+      </c>
+      <c r="C255" t="s">
+        <v>183</v>
+      </c>
+      <c r="D255" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A256" t="s">
+        <v>66</v>
+      </c>
+      <c r="B256">
         <v>4450</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C256" t="s">
+        <v>3</v>
+      </c>
+      <c r="D256" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A257" t="s">
+        <v>66</v>
+      </c>
+      <c r="B257">
+        <v>4450</v>
+      </c>
+      <c r="C257" t="s">
+        <v>3</v>
+      </c>
+      <c r="D257" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
+        <v>66</v>
+      </c>
+      <c r="B258">
+        <v>4450</v>
+      </c>
+      <c r="C258" t="s">
+        <v>3</v>
+      </c>
+      <c r="D258" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
+        <v>66</v>
+      </c>
+      <c r="B259">
+        <v>4450</v>
+      </c>
+      <c r="C259" t="s">
+        <v>10</v>
+      </c>
+      <c r="D259" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A260" t="s">
+        <v>66</v>
+      </c>
+      <c r="B260">
+        <v>4450</v>
+      </c>
+      <c r="C260" t="s">
+        <v>143</v>
+      </c>
+      <c r="D260" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
+        <v>66</v>
+      </c>
+      <c r="B261">
+        <v>4450</v>
+      </c>
+      <c r="C261" t="s">
         <v>145</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D261" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
+        <v>66</v>
+      </c>
+      <c r="B262">
+        <v>4450</v>
+      </c>
+      <c r="C262" t="s">
         <v>183</v>
+      </c>
+      <c r="D262" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>